<commit_message>
changed DB schema, added DOI column to Articles and in View table
</commit_message>
<xml_diff>
--- a/data/set_potato.xlsx
+++ b/data/set_potato.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="#ofTraitTables" sheetId="1" state="visible" r:id="rId2"/>
@@ -260,20 +260,22 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B2:B16 D1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9860465116279"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2186046511628"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7813953488372"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.25581395348837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3720930232558"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5860465116279"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1767441860465"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="9.05581395348837"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.25581395348837"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.05581395348837"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,18 +1100,19 @@
   </sheetPr>
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="1" sqref="B2:B16 C35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2697674418605"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0790697674419"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.25581395348837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.9441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3906976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.05581395348837"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2039,20 +2042,22 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.61395348837209"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.4744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.5348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="1017" min="9" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.25581395348837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.69302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.0046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.05581395348837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1906976744186"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1441860465116"/>
+    <col collapsed="false" hidden="false" max="1017" min="9" style="0" width="9.05581395348837"/>
+    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="9.25581395348837"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="23.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2536,22 +2541,22 @@
   </sheetPr>
   <dimension ref="A1:AMI37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.61395348837209"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="31.6418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="35.0139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="4.92093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.62790697674419"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="5.33953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="5.90697674418605"/>
-    <col collapsed="false" hidden="false" max="1023" min="9" style="5" width="22.3627906976744"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="14.0604651162791"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.25581395348837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.69302325581395"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="36.0325581395349"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="5.12093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="5.71162790697674"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="5.51162790697674"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="6.10232558139535"/>
+    <col collapsed="false" hidden="false" max="1023" min="9" style="5" width="23.0372093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="14.3720930232558"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="23.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2580,14 +2585,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
         <v>4354307</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>13</v>
       </c>
       <c r="D2" s="2" t="n">
@@ -3621,24 +3626,24 @@
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>
     </row>
-    <row r="3" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="n">
+    <row r="3" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>4374564</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>0</v>
+      <c r="C3" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
@@ -3646,16 +3651,20 @@
       <c r="H3" s="5" t="n">
         <v>0</v>
       </c>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="N3" s="0"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="n">
+    <row r="4" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>4448561</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D4" s="2" t="n">
@@ -3673,32 +3682,36 @@
       <c r="H4" s="5" t="n">
         <v>0</v>
       </c>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="N4" s="0"/>
       <c r="P4" s="2"/>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4551535</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>16</v>
+        <v>4480903</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>37</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I5" s="0"/>
       <c r="J5" s="0"/>
@@ -4716,21 +4729,21 @@
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>4551535</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F6" s="5" t="n">
         <v>0</v>
@@ -4739,7 +4752,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I6" s="0"/>
       <c r="J6" s="0"/>
@@ -5757,11 +5770,11 @@
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
         <v>4632055</v>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="2" t="n">
@@ -6798,14 +6811,14 @@
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="n">
         <v>4648990</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="3" t="n">
         <v>12</v>
       </c>
       <c r="D8" s="2" t="n">
@@ -7839,14 +7852,14 @@
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
     </row>
-    <row r="9" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="n">
+    <row r="9" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
         <v>4703618</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="0" t="n">
         <v>22</v>
       </c>
       <c r="D9" s="2" t="n">
@@ -7864,22 +7877,26 @@
       <c r="H9" s="5" t="n">
         <v>0</v>
       </c>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="N9" s="0"/>
     </row>
-    <row r="10" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
+    <row r="10" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
         <v>4773602</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>17</v>
+      <c r="C10" s="0" t="n">
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F10" s="5" t="n">
         <v>0</v>
@@ -7890,26 +7907,30 @@
       <c r="H10" s="5" t="n">
         <v>3</v>
       </c>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
+      <c r="N10" s="0"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>4799268</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="5" t="n">
-        <v>0</v>
+      <c r="C11" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>5</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F11" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>0</v>
@@ -8933,14 +8954,14 @@
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>4855764</v>
       </c>
-      <c r="B12" s="4" t="n">
+      <c r="B12" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="0" t="n">
         <v>43</v>
       </c>
       <c r="D12" s="2" t="n">
@@ -9974,21 +9995,21 @@
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>4900573</v>
       </c>
-      <c r="B13" s="4" t="n">
+      <c r="B13" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="0" t="n">
         <v>14</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F13" s="5" t="n">
         <v>0</v>
@@ -9997,7 +10018,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
@@ -11015,14 +11036,14 @@
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>5345157</v>
       </c>
-      <c r="B14" s="4" t="n">
+      <c r="B14" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="3" t="n">
         <v>7</v>
       </c>
       <c r="D14" s="5" t="n">
@@ -12056,14 +12077,14 @@
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>5567664</v>
       </c>
-      <c r="B15" s="4" t="n">
+      <c r="B15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="0" t="n">
         <v>11</v>
       </c>
       <c r="D15" s="2" t="n">
@@ -13097,15 +13118,15 @@
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="n">
         <v>3023753</v>
       </c>
-      <c r="B16" s="4" t="n">
+      <c r="B16" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="2" t="n">
-        <v>4</v>
+      <c r="C16" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>1</v>
@@ -14138,23 +14159,23 @@
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
     </row>
-    <row r="17" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="n">
         <f aca="false">SUM(C2:C16)</f>
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="D17" s="2" t="n">
         <f aca="false">SUM(D2:D16)</f>
-        <v>163</v>
+        <v>233</v>
       </c>
       <c r="E17" s="5" t="n">
         <f aca="false">SUM(E2:E16)</f>
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="F17" s="2" t="n">
         <f aca="false">SUM(F2:F16)</f>
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="G17" s="2" t="n">
         <f aca="false">SUM(G2:G16)</f>
@@ -14162,8 +14183,11 @@
       </c>
       <c r="H17" s="2" t="n">
         <f aca="false">SUM(H2:H16)</f>
-        <v>22</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
+      <c r="L17" s="0"/>
       <c r="P17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15203,11 +15227,11 @@
       <c r="B20" s="1"/>
       <c r="C20" s="3" t="n">
         <f aca="false">(E17/(E17+F17))</f>
-        <v>0.938650306748466</v>
+        <v>0.828193832599119</v>
       </c>
       <c r="D20" s="3" t="n">
         <f aca="false">(E17/(E17+H17))</f>
-        <v>0.874285714285714</v>
+        <v>0.959183673469388</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>

</xml_diff>